<commit_message>
Recursively print all sub sets
</commit_message>
<xml_diff>
--- a/Notes/SubSetSum problem.xlsx
+++ b/Notes/SubSetSum problem.xlsx
@@ -47,12 +47,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +383,7 @@
   <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,22 +422,22 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
+      <c r="B3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="b">
@@ -444,22 +451,22 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
+      <c r="B4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H4" t="b">
@@ -473,22 +480,22 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
+      <c r="B5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H5" t="b">
@@ -502,22 +509,22 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
+      <c r="B6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H6" t="b">

</xml_diff>